<commit_message>
EDIT Values of LED Resistors for 5mA
</commit_message>
<xml_diff>
--- a/TPS54302.xlsx
+++ b/TPS54302.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jamil\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jamil\Desktop\New folder (2)\RCS_AVR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0248CD49-4F1A-4A1C-B644-21B0400019AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0D0A282-2FB8-4E95-B8C1-C3DADC25D50A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>vref</t>
   </si>
@@ -106,13 +106,46 @@
   </si>
   <si>
     <t>سلف استاندارد شده</t>
+  </si>
+  <si>
+    <t>LED Resistors Calculate</t>
+  </si>
+  <si>
+    <t>GREEN</t>
+  </si>
+  <si>
+    <t>RED</t>
+  </si>
+  <si>
+    <t>Whaite</t>
+  </si>
+  <si>
+    <t>YELLOW</t>
+  </si>
+  <si>
+    <t>BLUE</t>
+  </si>
+  <si>
+    <t>TYPE</t>
+  </si>
+  <si>
+    <t>LED VOLTAGE</t>
+  </si>
+  <si>
+    <t>INPUT Current</t>
+  </si>
+  <si>
+    <t>Calculate Resistor</t>
+  </si>
+  <si>
+    <t>INPUT VOLTAGE LED</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -157,8 +190,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -173,6 +213,36 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -226,7 +296,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -263,6 +333,30 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="3" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="4" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -549,15 +643,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="26.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="11.140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="10.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="18.42578125" style="1" customWidth="1"/>
@@ -774,6 +868,122 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E22" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="F22" s="11"/>
+    </row>
+    <row r="24" spans="1:7" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" s="3"/>
+      <c r="C24" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D24" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="E24" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="F24" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="G24" s="17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" s="19"/>
+      <c r="C25" s="3">
+        <v>2</v>
+      </c>
+      <c r="D25" s="3">
+        <v>2</v>
+      </c>
+      <c r="E25" s="3">
+        <v>3</v>
+      </c>
+      <c r="F25" s="3">
+        <v>2</v>
+      </c>
+      <c r="G25" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26" s="19"/>
+      <c r="C26" s="3">
+        <v>5</v>
+      </c>
+      <c r="D26" s="3">
+        <v>5</v>
+      </c>
+      <c r="E26" s="3">
+        <v>3.3</v>
+      </c>
+      <c r="F26" s="3">
+        <v>12</v>
+      </c>
+      <c r="G26" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27" s="19"/>
+      <c r="C27" s="3">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D27" s="3">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E27" s="3">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F27" s="3">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G27" s="3">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="20"/>
+      <c r="C28" s="2">
+        <f>(C26-C25)/C27</f>
+        <v>600</v>
+      </c>
+      <c r="D28" s="2">
+        <f t="shared" ref="D28:G28" si="0">(D26-D25)/D27</f>
+        <v>600</v>
+      </c>
+      <c r="E28" s="2">
+        <f t="shared" si="0"/>
+        <v>59.999999999999964</v>
+      </c>
+      <c r="F28" s="2">
+        <f t="shared" si="0"/>
+        <v>2000</v>
+      </c>
+      <c r="G28" s="2">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>